<commit_message>
Allow static members to be dumped.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/InsertingData.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/InsertingData.xlsx
@@ -9,14 +9,14 @@
     <x:sheet name="Inserting Data" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Titles">'Inserting Data'!$A$1:$A$1,'Inserting Data'!$C$1:$H$1,'Inserting Data'!$A$6:$D$6,'Inserting Data'!$F$6:$H$6,'Inserting Data'!$F$13:$H$13</x:definedName>
+    <x:definedName name="Titles">'Inserting Data'!$A$1:$A$1,'Inserting Data'!$C$1:$H$1,'Inserting Data'!$A$6:$D$6,'Inserting Data'!$F$6:$H$6,'Inserting Data'!$F$11:$I$11,'Inserting Data'!$A$13:$C$13</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <x:si>
     <x:t>From Strings</x:t>
   </x:si>
@@ -84,7 +84,19 @@
     <x:t>Melanie</x:t>
   </x:si>
   <x:si>
+    <x:t>From List</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Person</x:t>
+  </x:si>
+  <x:si>
     <x:t>Transposed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>On Main St.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mary</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -466,7 +478,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:H16"/>
+  <x:dimension ref="A1:I16"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -474,14 +486,16 @@
   <x:cols>
     <x:col min="1" max="1" width="12.780625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.860625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="9.170625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.870625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="9.830625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="2.900625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="10.650625" style="0" customWidth="1"/>
-    <x:col min="7" max="8" width="11.870625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="11.850625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="11.870625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="3.960625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="7.720625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
+    <x:row r="1" spans="1:9">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -494,7 +508,7 @@
       <x:c r="G1" s="1" t="s"/>
       <x:c r="H1" s="1" t="s"/>
     </x:row>
-    <x:row r="2" spans="1:8">
+    <x:row r="2" spans="1:9">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
@@ -508,7 +522,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:8">
+    <x:row r="3" spans="1:9">
       <x:c r="A3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -516,7 +530,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:8">
+    <x:row r="4" spans="1:9">
       <x:c r="C4" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
@@ -536,7 +550,7 @@
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:8">
+    <x:row r="6" spans="1:9">
       <x:c r="A6" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -549,7 +563,7 @@
       <x:c r="G6" s="1" t="s"/>
       <x:c r="H6" s="1" t="s"/>
     </x:row>
-    <x:row r="7" spans="1:8">
+    <x:row r="7" spans="1:9">
       <x:c r="A7" s="0" t="n">
         <x:v>25</x:v>
       </x:c>
@@ -572,7 +586,7 @@
         <x:v>30</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:8">
+    <x:row r="8" spans="1:9">
       <x:c r="A8" s="0" t="n">
         <x:v>50</x:v>
       </x:c>
@@ -595,7 +609,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:8">
+    <x:row r="9" spans="1:9">
       <x:c r="A9" s="0" t="n">
         <x:v>10</x:v>
       </x:c>
@@ -618,7 +632,7 @@
         <x:v>45</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:8">
+    <x:row r="10" spans="1:9">
       <x:c r="A10" s="0" t="n">
         <x:v>21</x:v>
       </x:c>
@@ -632,7 +646,7 @@
         <x:v>36529</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:8">
+    <x:row r="11" spans="1:9">
       <x:c r="A11" s="0" t="n">
         <x:v>100</x:v>
       </x:c>
@@ -645,53 +659,110 @@
       <x:c r="D11" s="2">
         <x:v>36530</x:v>
       </x:c>
-    </x:row>
-    <x:row r="13" spans="1:8">
-      <x:c r="F13" s="1" t="s">
+      <x:c r="F11" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="G13" s="1" t="s"/>
-      <x:c r="H13" s="1" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:8">
+      <x:c r="G11" s="1" t="s"/>
+      <x:c r="H11" s="1" t="s"/>
+      <x:c r="I11" s="1" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:9">
+      <x:c r="F12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:9">
+      <x:c r="A13" s="1" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="1" t="s"/>
+      <x:c r="C13" s="1" t="s"/>
+      <x:c r="F13" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:9">
+      <x:c r="A14" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="H14" s="0" t="s">
+      <x:c r="H14" s="0" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:9">
+      <x:c r="A15" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-    </x:row>
-    <x:row r="15" spans="1:8">
-      <x:c r="F15" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="H15" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:8">
-      <x:c r="F16" s="0" t="n">
+      <x:c r="H15" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:9">
+      <x:c r="A16" s="0" t="n">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="G16" s="0" t="n">
+      <x:c r="B16" s="0" t="n">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="H16" s="0" t="n">
+      <x:c r="C16" s="0" t="n">
         <x:v>45</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="4">
+  <x:mergeCells count="5">
     <x:mergeCell ref="C1:H1"/>
     <x:mergeCell ref="A6:D6"/>
     <x:mergeCell ref="F6:H6"/>
-    <x:mergeCell ref="F13:H13"/>
+    <x:mergeCell ref="F11:I11"/>
+    <x:mergeCell ref="A13:C13"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>